<commit_message>
Adding more home page testcases
</commit_message>
<xml_diff>
--- a/utils/testcases-Zoom.xlsx
+++ b/utils/testcases-Zoom.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jyoti\Documents\Dev\zoom-automation-playwright\utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A6F48AF-0B53-42D5-B251-D13DD1FD84B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBA44D02-9A20-4C85-BB1D-D2BD770B5CBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>Sr no</t>
   </si>
@@ -312,6 +312,69 @@
   </si>
   <si>
     <t>User Profile</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Pre-requisite</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: user login
+1.In the right rail, click on Schedule present.
+2. Enter the meeting details and click Save.
+3. Go back to Home and observe the behavior.</t>
+    </r>
+  </si>
+  <si>
+    <t>1. The top card should contain details like Schedule, Join and Host meetings and Personal meeting ID.
+1.1 Clicking on Schedule, should open PERSONAL -&gt; Meetings page to schedule meeting in a new tab.
+2. Meeting should be created.
+3. Meeting card present in right rail, Home page should contain the scheduled meeting info.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Pre-requisite</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: user login
+1. In the right rail, click on 'Join' present.
+2. Enter the meeting ID/ link name or personal meeting id to start the meeting.
+3. Click on Join.
+4. A pop-up to open Zoom desktop app should show, click on Cancel.
+5. Click on Launch Meeting button present.
+6. Repeat step 4.
+7. Click on 'Join from your browser'..
+8. Obseve the behavior.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -439,6 +502,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -449,21 +527,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -758,42 +821,42 @@
   <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A11" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:E19"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="5.53515625" style="6" customWidth="1"/>
     <col min="2" max="2" width="45.07421875" style="4" customWidth="1"/>
-    <col min="3" max="3" width="61.07421875" style="13" customWidth="1"/>
+    <col min="3" max="3" width="61.07421875" style="9" customWidth="1"/>
     <col min="4" max="4" width="50.765625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="11" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
     </row>
     <row r="3" spans="1:5" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A3" s="5">
@@ -802,7 +865,7 @@
       <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="8" t="s">
         <v>8</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -817,7 +880,7 @@
       <c r="B4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="8" t="s">
         <v>9</v>
       </c>
       <c r="D4" s="2" t="s">
@@ -826,13 +889,13 @@
       <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="10"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="15"/>
     </row>
     <row r="6" spans="1:5" ht="255.45" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="5">
@@ -841,7 +904,7 @@
       <c r="B6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="8" t="s">
         <v>13</v>
       </c>
       <c r="D6" s="3" t="s">
@@ -856,7 +919,7 @@
       <c r="B7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="8" t="s">
         <v>17</v>
       </c>
       <c r="D7" s="2" t="s">
@@ -871,7 +934,7 @@
       <c r="B8" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="8" t="s">
         <v>26</v>
       </c>
       <c r="D8" s="2" t="s">
@@ -886,7 +949,7 @@
       <c r="B9" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="8" t="s">
         <v>21</v>
       </c>
       <c r="D9" s="2" t="s">
@@ -901,7 +964,7 @@
       <c r="B10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="8" t="s">
         <v>24</v>
       </c>
       <c r="D10" s="2" t="s">
@@ -916,7 +979,7 @@
       <c r="B11" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="8" t="s">
         <v>28</v>
       </c>
       <c r="D11" s="2" t="s">
@@ -924,25 +987,31 @@
       </c>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:5" ht="102" x14ac:dyDescent="0.4">
       <c r="A12" s="5">
         <v>9</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="12"/>
-      <c r="D12" s="2"/>
+      <c r="C12" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:5" ht="145.75" x14ac:dyDescent="0.4">
       <c r="A13" s="5">
         <v>10</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="12"/>
+      <c r="C13" s="8" t="s">
+        <v>41</v>
+      </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
     </row>
@@ -953,7 +1022,7 @@
       <c r="B14" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="12"/>
+      <c r="C14" s="8"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
     </row>
@@ -964,7 +1033,7 @@
       <c r="B15" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="12"/>
+      <c r="C15" s="8"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
     </row>
@@ -975,7 +1044,7 @@
       <c r="B16" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C16" s="12"/>
+      <c r="C16" s="8"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
     </row>
@@ -986,7 +1055,7 @@
       <c r="B17" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C17" s="12"/>
+      <c r="C17" s="8"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
@@ -997,7 +1066,7 @@
       <c r="B18" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C18" s="12"/>
+      <c r="C18" s="8"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
     </row>
@@ -1015,7 +1084,7 @@
         <v>16</v>
       </c>
       <c r="B20" s="3"/>
-      <c r="C20" s="12"/>
+      <c r="C20" s="8"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
     </row>
@@ -1024,7 +1093,7 @@
         <v>17</v>
       </c>
       <c r="B21" s="3"/>
-      <c r="C21" s="12"/>
+      <c r="C21" s="8"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
     </row>
@@ -1033,7 +1102,7 @@
         <v>18</v>
       </c>
       <c r="B22" s="3"/>
-      <c r="C22" s="12"/>
+      <c r="C22" s="8"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
     </row>
@@ -1042,7 +1111,7 @@
         <v>19</v>
       </c>
       <c r="B23" s="3"/>
-      <c r="C23" s="12"/>
+      <c r="C23" s="8"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
     </row>
@@ -1051,7 +1120,7 @@
         <v>20</v>
       </c>
       <c r="B24" s="3"/>
-      <c r="C24" s="12"/>
+      <c r="C24" s="8"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
     </row>
@@ -1060,7 +1129,7 @@
         <v>21</v>
       </c>
       <c r="B25" s="3"/>
-      <c r="C25" s="12"/>
+      <c r="C25" s="8"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
     </row>
@@ -1069,7 +1138,7 @@
         <v>22</v>
       </c>
       <c r="B26" s="3"/>
-      <c r="C26" s="12"/>
+      <c r="C26" s="8"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
     </row>
@@ -1078,7 +1147,7 @@
         <v>23</v>
       </c>
       <c r="B27" s="3"/>
-      <c r="C27" s="12"/>
+      <c r="C27" s="8"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
     </row>
@@ -1087,7 +1156,7 @@
         <v>24</v>
       </c>
       <c r="B28" s="3"/>
-      <c r="C28" s="12"/>
+      <c r="C28" s="8"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
     </row>
@@ -1096,7 +1165,7 @@
         <v>25</v>
       </c>
       <c r="B29" s="3"/>
-      <c r="C29" s="12"/>
+      <c r="C29" s="8"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
     </row>
@@ -1105,7 +1174,7 @@
         <v>26</v>
       </c>
       <c r="B30" s="3"/>
-      <c r="C30" s="12"/>
+      <c r="C30" s="8"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
     </row>

</xml_diff>

<commit_message>
more zoom home test
</commit_message>
<xml_diff>
--- a/utils/testcases-Zoom.xlsx
+++ b/utils/testcases-Zoom.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jyoti\Documents\Dev\zoom-automation-playwright\utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBA44D02-9A20-4C85-BB1D-D2BD770B5CBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53553587-0B80-4ED0-8A02-E821271B8666}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t>Sr no</t>
   </si>
@@ -73,6 +73,345 @@
   </si>
   <si>
     <t>Verify user can navigate to non-admin tiles present in left rail (Home, Profile, Meetings, Webinars, Events &amp; Sessions, Personal Contacts, Personal Devices, Whiteboards, Notes, Docs, Recording, Clips, Scheduler, Settings, Data &amp; Privacy, and Reports)</t>
+  </si>
+  <si>
+    <t>Clicking on tile, should get highlighted in left rail.</t>
+  </si>
+  <si>
+    <t>Zoom Home</t>
+  </si>
+  <si>
+    <t>Verify left rail section</t>
+  </si>
+  <si>
+    <t>2. There should be two sections in left rail "PERSONAL" and "ADMIN" and three links "Zoom learning section", "Video Tutorials", and "Knowledge Base" at the bottom</t>
+  </si>
+  <si>
+    <t>[Zoom-Home] User info card (Username, current plan, Job title, Iincluded in plan, etc)</t>
+  </si>
+  <si>
+    <t>[Zoom-Home] Discover our other popular products</t>
+  </si>
+  <si>
+    <t>2. By-default three Zoom prodcuts should show under "Discover our other products" .
+2.2. 'View more products' toggle should show beneath the default 3 products list
+4. Other available products should show on the same page--without page refresh.</t>
+  </si>
+  <si>
+    <t>[Zoom-Home] Your Activity</t>
+  </si>
+  <si>
+    <t>2. By default three activity tile or suggestion tile should show under "Your Activitys" block.
+3. Clicking toggle should expand/collapse the corresponding activity.</t>
+  </si>
+  <si>
+    <t>1. User name, job title, Plan details and manage plan button should be avaialble in user info card post login.
+2. Manage Plan should redirect user to ADMIN (left rail) -&gt; Plans and Billing -&gt; Plan Management page.
+3. View Plan Details should open a new flyout with "View all plans" and "Upgrade Now" buttons.</t>
+  </si>
+  <si>
+    <t>[Zoom-Home] Your Activity Default view, verify if no activity is performed, every tile details should have Learn more and Create [Activity_Name] button present along with Visit [Activity_Name] link.</t>
+  </si>
+  <si>
+    <t>5. Learns more should redirect user to activity doc</t>
+  </si>
+  <si>
+    <t>[Zoom-Home] Schedule meeting from Home</t>
+  </si>
+  <si>
+    <t>[Zoom-Home] Join meeting from Home</t>
+  </si>
+  <si>
+    <t>[Zoom-Home] Host meeting from Home</t>
+  </si>
+  <si>
+    <t>Verify right rail section contains Personal Meeting ID information, Meetings details, Plan benefits, Ad Carousel, and card containing links to Explore, Resources, and QnA (5 sections).</t>
+  </si>
+  <si>
+    <t>[Zoom-Home] Verify then copy personal meeting id</t>
+  </si>
+  <si>
+    <t>User Profile</t>
+  </si>
+  <si>
+    <t>1. The top card should contain details like Schedule, Join and Host meetings and Personal meeting ID.
+1.1 Clicking on Schedule, should open PERSONAL -&gt; Meetings page to schedule meeting in a new tab.
+2. Meeting should be created.
+3. Meeting card present in right rail, Home page should contain the scheduled meeting info.</t>
+  </si>
+  <si>
+    <t>1. The top card should contain details like Schedule, Join and Host meetings and Personal meeting ID.
+3. Clicking on Join, should open a new tab to join a meeting.
+5.After user clicks cancel in the popup, then Launch Meeting button, "join from browser" button should appear on the page
+7. Meeting should be joined.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Pre-requisite</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: user login
+1. In the right rail, click on 'Host' present.
+2. Click on Launch Meeting button present.
+3. A pop-up to open Zoom desktop app should show, click on Cancel.
+4. Click on 'Join from your browser'.
+5. Obseve the behavior.</t>
+    </r>
+  </si>
+  <si>
+    <t>1. The top card should contain details like Schedule, Join and Host meetings and Personal meeting ID.
+1.1 Clicking on Host, should open a new tab to join a meeting.
+2. After user clicks the Launch Meeting button, "join from browser" button should appear on the page.
+4. Meeting should be joined.</t>
+  </si>
+  <si>
+    <t>Right rail section should contain Personal Meeting ID information, Meetings details, Plan benefits, Ad Carousel, and card containing links to Explore, Resources, and QnA (5 sections).</t>
+  </si>
+  <si>
+    <t>3. A pop-up informing user "Copied to clipboard" should show up for 3-5 seconds.</t>
+  </si>
+  <si>
+    <t>User should be able to test Audio and Video from Home</t>
+  </si>
+  <si>
+    <t>[Zoom-Home] Verify user is able to test Audio and Video from Home</t>
+  </si>
+  <si>
+    <t>[Zoom-Home] Verify user is able to navigate to meeting details</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Pre-requisite</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: a. user login
+b. there should be zero meeting present in Meetings card.
+1. In the right rail, second card should show information of available meetings and a button to test audio and video.
+2. Click "Test Audio and Video" button present.
+3. A new page asking user to join a test meeting should load, click on "Join".
+4. Click "Launch Meeting", a prompt asking user to open desktop app should load, click on cancel then click on "Join from your browser" link below the Launch Meeting button.
+5. In the pre-join screen enter User name, then click Join.
+6. Click "Start Video" button present, select camera then click Yes.
+7. Select audio and then click Yes followed by Microphone and 'Yes'.
+8. After the test, click End Test.
+9. Obseve the behavior.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Pre-requisite</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: user login
+1. In the right rail, top card Personal Meeting ID should be present.
+2. Click copy icon present next to Personal Meeting ID.
+3. Obseve the behavior.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Pre-requisite</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: user login
+1. Scroll the right rail to observe availble cards.
+2. Verify if 5 cards appear.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Pre-requisite</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: user login
+1. Scroll down the home page to "Your Activity".
+2. Observe if default three activity or suggestion shows up in "Your Activity section" with toggle to expand and collapse details.
+3. Click on the toggle present to expand any of the activity, if not already expanded.
+4. Observe the behavior.
+5. Click on "Learn More".
+6. Go back to Home -&gt; Your Activity</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Pre-requisite</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: user login
+1. Scroll down the home page to "Your Activity".
+2. Observe if default three activity or suggestion shows up in "Your Activity section" with toggle to expand and collapse details.
+3. Click on the toggle present to any of the activity, observe the behavior.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Pre-requisite</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: user login
+1. Scroll down the home page to "Discover our other popular products".
+2. Observe if default three Zoom products show up on page with 'View more products" toggle link.
+3. Click on 'View more products' toggle.
+4. Observe the behavior.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Pre-requisite</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: user login
+1. By default home tile in left rail should be active, verify the user details and plan details.
+2. Click on Manage Plan, observe the behavior.
+3. Go back to Home and click on 'View Plan Details' link.
+4. Observe the behavior.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Pre-requisite</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: user login
+1. By default home tile in left rail should be active.
+2. Scroll down in the left rail.
+3. Observe the section headings.</t>
+    </r>
   </si>
   <si>
     <r>
@@ -114,238 +453,6 @@
     </r>
   </si>
   <si>
-    <t>Clicking on tile, should get highlighted in left rail.</t>
-  </si>
-  <si>
-    <t>Zoom Home</t>
-  </si>
-  <si>
-    <t>Verify left rail section</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Pre-requisite</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: user login
-1. By default home tile in left rail should be active.
-2. Scroll down in the left rail.
-3. Observe the section headings.</t>
-    </r>
-  </si>
-  <si>
-    <t>2. There should be two sections in left rail "PERSONAL" and "ADMIN" and three links "Zoom learning section", "Video Tutorials", and "Knowledge Base" at the bottom</t>
-  </si>
-  <si>
-    <t>[Zoom-Home] User info card (Username, current plan, Job title, Iincluded in plan, etc)</t>
-  </si>
-  <si>
-    <t>[Zoom-Home] Discover our other popular products</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Pre-requisite</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: user login
-1. Scroll down the home page to "Discover our other popular products".
-2. Observe if default three Zoom products show up on page with 'View more products" toggle link.
-3. Click on 'View more products' toggle.
-4. Observe the behavior.</t>
-    </r>
-  </si>
-  <si>
-    <t>2. By-default three Zoom prodcuts should show under "Discover our other products" .
-2.2. 'View more products' toggle should show beneath the default 3 products list
-4. Other available products should show on the same page--without page refresh.</t>
-  </si>
-  <si>
-    <t>[Zoom-Home] Your Activity</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Pre-requisite</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: user login
-1. Scroll down the home page to "Your Activity".
-2. Observe if default three activity or suggestion shows up in "Your Activity section" with toggle to expand and collapse details.
-3. Click on the toggle present to any of the activity, observe the behavior.</t>
-    </r>
-  </si>
-  <si>
-    <t>2. By default three activity tile or suggestion tile should show under "Your Activitys" block.
-3. Clicking toggle should expand/collapse the corresponding activity.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Pre-requisite</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: user login
-1. By default home tile in left rail should be active, verify the user details and plan details.
-2. Click on Manage Plan, observe the behavior.
-3. Go back to Home and click on 'View Plan Details' link.
-4. Observe the behavior.</t>
-    </r>
-  </si>
-  <si>
-    <t>1. User name, job title, Plan details and manage plan button should be avaialble in user info card post login.
-2. Manage Plan should redirect user to ADMIN (left rail) -&gt; Plans and Billing -&gt; Plan Management page.
-3. View Plan Details should open a new flyout with "View all plans" and "Upgrade Now" buttons.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Pre-requisite</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: user login
-1. Scroll down the home page to "Your Activity".
-2. Observe if default three activity or suggestion shows up in "Your Activity section" with toggle to expand and collapse details.
-3. Click on the toggle present to expand any of the activity, if not already expanded.
-4. Observe the behavior.
-5. Click on "Learn More".
-6. Go back to Home -&gt; Your Activity</t>
-    </r>
-  </si>
-  <si>
-    <t>[Zoom-Home] Your Activity Default view, verify if no activity is performed, every tile details should have Learn more and Create [Activity_Name] button present along with Visit [Activity_Name] link.</t>
-  </si>
-  <si>
-    <t>5. Learns more should redirect user to activity doc</t>
-  </si>
-  <si>
-    <t>[Zoom-Home] Schedule meeting from Home</t>
-  </si>
-  <si>
-    <t>[Zoom-Home] Join meeting from Home</t>
-  </si>
-  <si>
-    <t>[Zoom-Home] Host meeting from Home</t>
-  </si>
-  <si>
-    <t>Verify right rail section contains Personal Meeting ID information, Meetings details, Plan benefits, Ad Carousel, and card containing links to Explore, Resources, and QnA (5 sections).</t>
-  </si>
-  <si>
-    <t>[Zoom-Home] Verify then copy personal meeting id</t>
-  </si>
-  <si>
-    <t>[Zoom-Home] Verify user is able to test Audio and Video from Home page itself</t>
-  </si>
-  <si>
-    <t>[Zoom-Home] Verify user is able to navigate to meeting details from Home page itself</t>
-  </si>
-  <si>
-    <t>User Profile</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Pre-requisite</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: user login
-1.In the right rail, click on Schedule present.
-2. Enter the meeting details and click Save.
-3. Go back to Home and observe the behavior.</t>
-    </r>
-  </si>
-  <si>
-    <t>1. The top card should contain details like Schedule, Join and Host meetings and Personal meeting ID.
-1.1 Clicking on Schedule, should open PERSONAL -&gt; Meetings page to schedule meeting in a new tab.
-2. Meeting should be created.
-3. Meeting card present in right rail, Home page should contain the scheduled meeting info.</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -375,6 +482,35 @@
 7. Click on 'Join from your browser'..
 8. Obseve the behavior.</t>
     </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Pre-requisite</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: user login
+1.In the right rail, click on Schedule present.
+2. Enter the meeting details and click Save.
+3. Go back to Home and observe the behavior.</t>
+    </r>
+  </si>
+  <si>
+    <t>[Zoom-Home] Verify if any meetings is present, user can copy invitation and navigate to meeting information from Meetings card itself, right rail.</t>
   </si>
 </sst>
 </file>
@@ -820,8 +956,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -829,7 +965,7 @@
     <col min="1" max="1" width="5.53515625" style="6" customWidth="1"/>
     <col min="2" max="2" width="45.07421875" style="4" customWidth="1"/>
     <col min="3" max="3" width="61.07421875" style="9" customWidth="1"/>
-    <col min="4" max="4" width="50.765625" customWidth="1"/>
+    <col min="4" max="4" width="50.765625" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.4">
@@ -842,7 +978,7 @@
       <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="11" t="s">
@@ -868,7 +1004,7 @@
       <c r="C3" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="2"/>
@@ -883,21 +1019,21 @@
       <c r="C4" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A5" s="13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5" s="14"/>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
       <c r="E5" s="15"/>
     </row>
-    <row r="6" spans="1:5" ht="255.45" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:5" ht="265.3" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="5">
         <v>3</v>
       </c>
@@ -905,85 +1041,85 @@
         <v>12</v>
       </c>
       <c r="C6" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>14</v>
-      </c>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:5" ht="58.3" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:5" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A7" s="5">
         <v>4</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="E7" s="2"/>
     </row>
-    <row r="8" spans="1:5" ht="87.45" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:5" ht="102" x14ac:dyDescent="0.4">
       <c r="A8" s="5">
         <v>5</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>27</v>
+        <v>46</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:5" ht="87.45" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:5" ht="102" x14ac:dyDescent="0.4">
       <c r="A9" s="5">
         <v>6</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>22</v>
+        <v>45</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="E9" s="2"/>
     </row>
-    <row r="10" spans="1:5" ht="87.45" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:5" ht="102" x14ac:dyDescent="0.4">
       <c r="A10" s="5">
         <v>7</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>25</v>
+        <v>44</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:5" ht="131.15" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:5" ht="145.75" x14ac:dyDescent="0.4">
       <c r="A11" s="5">
         <v>8</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>30</v>
+        <v>43</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>24</v>
       </c>
       <c r="E11" s="2"/>
     </row>
@@ -992,38 +1128,44 @@
         <v>9</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>40</v>
-      </c>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:5" ht="145.75" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:5" ht="160.30000000000001" x14ac:dyDescent="0.4">
       <c r="A13" s="5">
         <v>10</v>
       </c>
       <c r="B13" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="D13" s="2"/>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:5" ht="102" x14ac:dyDescent="0.4">
       <c r="A14" s="5">
         <v>11</v>
       </c>
       <c r="B14" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="2"/>
+      <c r="D14" s="3" t="s">
+        <v>34</v>
+      </c>
       <c r="E14" s="2"/>
     </row>
     <row r="15" spans="1:5" ht="58.3" x14ac:dyDescent="0.4">
@@ -1031,32 +1173,44 @@
         <v>12</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C15" s="8"/>
-      <c r="D15" s="2"/>
+        <v>28</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>35</v>
+      </c>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:5" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A16" s="5">
         <v>13</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C16" s="8"/>
-      <c r="D16" s="2"/>
+        <v>29</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>36</v>
+      </c>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:5" ht="233.15" x14ac:dyDescent="0.4">
       <c r="A17" s="5">
         <v>14</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C17" s="8"/>
-      <c r="D17" s="2"/>
+        <v>38</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>37</v>
+      </c>
       <c r="E17" s="2"/>
     </row>
     <row r="18" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
@@ -1064,29 +1218,31 @@
         <v>15</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C18" s="8"/>
-      <c r="D18" s="2"/>
+      <c r="D18" s="3"/>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A19" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="B19" s="17"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="18"/>
+    <row r="19" spans="1:5" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A19" s="5">
+        <v>16</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" s="8"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="2"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A20" s="5">
-        <v>16</v>
-      </c>
-      <c r="B20" s="3"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
+      <c r="A20" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" s="17"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="18"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A21" s="5">
@@ -1094,7 +1250,7 @@
       </c>
       <c r="B21" s="3"/>
       <c r="C21" s="8"/>
-      <c r="D21" s="2"/>
+      <c r="D21" s="3"/>
       <c r="E21" s="2"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.4">
@@ -1103,7 +1259,7 @@
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="8"/>
-      <c r="D22" s="2"/>
+      <c r="D22" s="3"/>
       <c r="E22" s="2"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.4">
@@ -1112,7 +1268,7 @@
       </c>
       <c r="B23" s="3"/>
       <c r="C23" s="8"/>
-      <c r="D23" s="2"/>
+      <c r="D23" s="3"/>
       <c r="E23" s="2"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.4">
@@ -1121,7 +1277,7 @@
       </c>
       <c r="B24" s="3"/>
       <c r="C24" s="8"/>
-      <c r="D24" s="2"/>
+      <c r="D24" s="3"/>
       <c r="E24" s="2"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.4">
@@ -1130,7 +1286,7 @@
       </c>
       <c r="B25" s="3"/>
       <c r="C25" s="8"/>
-      <c r="D25" s="2"/>
+      <c r="D25" s="3"/>
       <c r="E25" s="2"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.4">
@@ -1139,7 +1295,7 @@
       </c>
       <c r="B26" s="3"/>
       <c r="C26" s="8"/>
-      <c r="D26" s="2"/>
+      <c r="D26" s="3"/>
       <c r="E26" s="2"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.4">
@@ -1148,7 +1304,7 @@
       </c>
       <c r="B27" s="3"/>
       <c r="C27" s="8"/>
-      <c r="D27" s="2"/>
+      <c r="D27" s="3"/>
       <c r="E27" s="2"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.4">
@@ -1157,7 +1313,7 @@
       </c>
       <c r="B28" s="3"/>
       <c r="C28" s="8"/>
-      <c r="D28" s="2"/>
+      <c r="D28" s="3"/>
       <c r="E28" s="2"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.4">
@@ -1166,7 +1322,7 @@
       </c>
       <c r="B29" s="3"/>
       <c r="C29" s="8"/>
-      <c r="D29" s="2"/>
+      <c r="D29" s="3"/>
       <c r="E29" s="2"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.4">
@@ -1175,14 +1331,14 @@
       </c>
       <c r="B30" s="3"/>
       <c r="C30" s="8"/>
-      <c r="D30" s="2"/>
+      <c r="D30" s="3"/>
       <c r="E30" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="A5:E5"/>
-    <mergeCell ref="A19:E19"/>
+    <mergeCell ref="A20:E20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added final home testcases
</commit_message>
<xml_diff>
--- a/utils/testcases-Zoom.xlsx
+++ b/utils/testcases-Zoom.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jyoti\Documents\Dev\zoom-automation-playwright\utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53553587-0B80-4ED0-8A02-E821271B8666}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F31AB77A-9A69-4333-B9E3-C8653A0671B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
   <si>
     <t>Sr no</t>
   </si>
@@ -511,6 +511,69 @@
   </si>
   <si>
     <t>[Zoom-Home] Verify if any meetings is present, user can copy invitation and navigate to meeting information from Meetings card itself, right rail.</t>
+  </si>
+  <si>
+    <t>3. Meetings in left rail PERSONAL -&gt; Meetings should be highlighted.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Pre-requisite</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: user login
+1. In the right rail, second card should show information of available meetings and a button to test audio and video.
+2. Click "Visit Meetings" link present.
+3. Obseve the behavior.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Pre-requisite</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: a. user login
+b. there should be alteast one meeting showing up in Meetings card.
+1. In the right rail, second card should show information of available meetings and a button to test audio and video.
+2. In the listed meetings, click on Copy meetign invitation,  a fly-out will show, click on Copy Meeting invitation.
+3. Obseve the behavior.
+4. Go back to Zoom Home page, click on the meeting title link, observe the behavior.
+5. Click on Start meeting, observe the behavior.</t>
+    </r>
+  </si>
+  <si>
+    <t>3. A pop-up informing user "Copied to clipboard" should show up for 3-5 seconds.
+4. Meeting detail page should open.
+5. User should be navigated to launch meeting page with "Launch Meeting" button present.</t>
   </si>
 </sst>
 </file>
@@ -956,8 +1019,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1213,26 +1276,34 @@
       </c>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:5" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A18" s="5">
         <v>15</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C18" s="8"/>
-      <c r="D18" s="3"/>
+      <c r="C18" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>52</v>
+      </c>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="1:5" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:5" ht="160.30000000000001" x14ac:dyDescent="0.4">
       <c r="A19" s="5">
         <v>16</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C19" s="8"/>
-      <c r="D19" s="3"/>
+      <c r="C19" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="E19" s="2"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
minor column updates in testcases sheet
</commit_message>
<xml_diff>
--- a/utils/testcases-Zoom.xlsx
+++ b/utils/testcases-Zoom.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jyoti\Documents\Dev\zoom-automation-playwright\utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F31AB77A-9A69-4333-B9E3-C8653A0671B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC122CFB-D73C-4BEF-B7FF-43A309F5D1E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,9 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
   <si>
-    <t>Sr no</t>
-  </si>
-  <si>
     <t>Title</t>
   </si>
   <si>
@@ -574,6 +571,9 @@
     <t>3. A pop-up informing user "Copied to clipboard" should show up for 3-5 seconds.
 4. Meeting detail page should open.
 5. User should be navigated to launch meeting page with "Launch Meeting" button present.</t>
+  </si>
+  <si>
+    <t>TC id</t>
   </si>
 </sst>
 </file>
@@ -1019,9 +1019,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:E20"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
@@ -1033,24 +1031,24 @@
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="C1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="D1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="E1" s="11" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A2" s="12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
@@ -1062,13 +1060,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E3" s="2"/>
     </row>
@@ -1077,19 +1075,19 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>10</v>
       </c>
       <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A5" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" s="14"/>
       <c r="C5" s="14"/>
@@ -1101,13 +1099,13 @@
         <v>3</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>12</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>13</v>
       </c>
       <c r="E6" s="2"/>
     </row>
@@ -1116,13 +1114,13 @@
         <v>4</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>16</v>
       </c>
       <c r="E7" s="2"/>
     </row>
@@ -1131,13 +1129,13 @@
         <v>5</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E8" s="2"/>
     </row>
@@ -1146,13 +1144,13 @@
         <v>6</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>19</v>
       </c>
       <c r="E9" s="2"/>
     </row>
@@ -1161,13 +1159,13 @@
         <v>7</v>
       </c>
       <c r="B10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>21</v>
       </c>
       <c r="E10" s="2"/>
     </row>
@@ -1176,13 +1174,13 @@
         <v>8</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>24</v>
       </c>
       <c r="E11" s="2"/>
     </row>
@@ -1191,13 +1189,13 @@
         <v>9</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E12" s="2"/>
     </row>
@@ -1206,13 +1204,13 @@
         <v>10</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E13" s="2"/>
     </row>
@@ -1221,13 +1219,13 @@
         <v>11</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C14" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>34</v>
       </c>
       <c r="E14" s="2"/>
     </row>
@@ -1236,13 +1234,13 @@
         <v>12</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E15" s="2"/>
     </row>
@@ -1251,13 +1249,13 @@
         <v>13</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E16" s="2"/>
     </row>
@@ -1266,13 +1264,13 @@
         <v>14</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E17" s="2"/>
     </row>
@@ -1281,13 +1279,13 @@
         <v>15</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E18" s="2"/>
     </row>
@@ -1296,19 +1294,19 @@
         <v>16</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C19" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D19" s="3" t="s">
         <v>54</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>55</v>
       </c>
       <c r="E19" s="2"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A20" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B20" s="17"/>
       <c r="C20" s="17"/>

</xml_diff>

<commit_message>
minor modifications to testcases
</commit_message>
<xml_diff>
--- a/utils/testcases-Zoom.xlsx
+++ b/utils/testcases-Zoom.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jyoti\Documents\Dev\zoom-automation-playwright\utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC122CFB-D73C-4BEF-B7FF-43A309F5D1E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E68F2755-FFBC-40F0-AB12-A571252EA023}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,12 +42,6 @@
     <t>Zoom login</t>
   </si>
   <si>
-    <t>Verify user signin with email/password-successful signin</t>
-  </si>
-  <si>
-    <t>Verify error details when user signs in with email/password-incorrect credentials</t>
-  </si>
-  <si>
     <t>1. Open browser and navigate to "https://zoom.com/signin".
 2. Type user email in 'Email Adress' field and password in "Password" field.
 3. Click on "Sign In" button present.</t>
@@ -574,6 +568,12 @@
   </si>
   <si>
     <t>TC id</t>
+  </si>
+  <si>
+    <t>[successful Authentication] Verify user signin with email/password</t>
+  </si>
+  <si>
+    <t>[Negative Test] Verify error details when user signs in with email/password-incorrect credentials</t>
   </si>
 </sst>
 </file>
@@ -1019,7 +1019,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
@@ -1031,7 +1033,7 @@
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B1" s="10" t="s">
         <v>0</v>
@@ -1060,13 +1062,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>7</v>
-      </c>
       <c r="D3" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E3" s="2"/>
     </row>
@@ -1075,19 +1077,19 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>8</v>
-      </c>
       <c r="D4" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A5" s="13" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B5" s="14"/>
       <c r="C5" s="14"/>
@@ -1099,13 +1101,13 @@
         <v>3</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E6" s="2"/>
     </row>
@@ -1114,13 +1116,13 @@
         <v>4</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E7" s="2"/>
     </row>
@@ -1129,13 +1131,13 @@
         <v>5</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E8" s="2"/>
     </row>
@@ -1144,13 +1146,13 @@
         <v>6</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E9" s="2"/>
     </row>
@@ -1159,13 +1161,13 @@
         <v>7</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E10" s="2"/>
     </row>
@@ -1174,13 +1176,13 @@
         <v>8</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E11" s="2"/>
     </row>
@@ -1189,13 +1191,13 @@
         <v>9</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E12" s="2"/>
     </row>
@@ -1204,13 +1206,13 @@
         <v>10</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E13" s="2"/>
     </row>
@@ -1219,13 +1221,13 @@
         <v>11</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E14" s="2"/>
     </row>
@@ -1234,13 +1236,13 @@
         <v>12</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E15" s="2"/>
     </row>
@@ -1249,13 +1251,13 @@
         <v>13</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E16" s="2"/>
     </row>
@@ -1264,13 +1266,13 @@
         <v>14</v>
       </c>
       <c r="B17" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="8" t="s">
-        <v>39</v>
-      </c>
       <c r="D17" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E17" s="2"/>
     </row>
@@ -1279,13 +1281,13 @@
         <v>15</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E18" s="2"/>
     </row>
@@ -1294,19 +1296,19 @@
         <v>16</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E19" s="2"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A20" s="16" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B20" s="17"/>
       <c r="C20" s="17"/>

</xml_diff>